<commit_message>
ship level and remove stupid one block levels
</commit_message>
<xml_diff>
--- a/tools/map_sheet.xlsx
+++ b/tools/map_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="27660" windowHeight="12915"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="2">
   <si>
     <t>b3</t>
   </si>
   <si>
-    <t>a1</t>
+    <t>c2</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,84 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF008000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3399FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6600FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -79,161 +156,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3399FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF008000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF00FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6600FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0000FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3399FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF008000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFC07F00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -241,6 +164,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC07F00"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF6600FF"/>
       <color rgb="FF0000FF"/>
@@ -552,15 +476,13 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="17" width="4.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="4.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
+    <col min="2" max="19" width="4.5703125" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -628,21 +550,20 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>0</v>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>0</v>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <v>41</v>
+      </c>
+      <c r="M2" s="2">
+        <v>41</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -659,26 +580,31 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
       <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2">
-        <v>11</v>
+      <c r="I3" s="2">
+        <v>1</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2">
-        <v>21</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="M3" s="2">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2">
+        <v>41</v>
+      </c>
+      <c r="O3" s="2">
+        <v>41</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -690,29 +616,37 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
       <c r="I4" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="2">
-        <v>21</v>
-      </c>
-      <c r="L4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>41</v>
+      </c>
       <c r="M4" s="2">
         <v>41</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2" t="s">
-        <v>0</v>
+      <c r="N4" s="2">
+        <v>41</v>
+      </c>
+      <c r="O4" s="2">
+        <v>41</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -725,33 +659,39 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2">
+        <v>11</v>
+      </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
       <c r="H5" s="2">
-        <v>11</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2">
         <v>41</v>
       </c>
-      <c r="M5" s="2"/>
+      <c r="M5" s="2">
+        <v>41</v>
+      </c>
       <c r="N5" s="2">
-        <v>51</v>
-      </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="O5" s="2">
+        <v>41</v>
+      </c>
+      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -762,34 +702,48 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2"/>
+      <c r="D6" s="2">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2">
+        <v>11</v>
+      </c>
       <c r="F6" s="2">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
       <c r="H6" s="2">
-        <v>21</v>
-      </c>
-      <c r="I6" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
       <c r="J6" s="2">
-        <v>41</v>
-      </c>
-      <c r="K6" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
       <c r="L6" s="2">
-        <v>51</v>
-      </c>
-      <c r="M6" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="M6" s="2">
+        <v>41</v>
+      </c>
       <c r="N6" s="2">
-        <v>61</v>
-      </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="O6" s="2">
+        <v>41</v>
+      </c>
+      <c r="P6" s="2">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>41</v>
+      </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
@@ -797,38 +751,38 @@
       <c r="A7" s="1">
         <v>28</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2"/>
+      <c r="B7" s="2">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>11</v>
+      </c>
       <c r="E7" s="2">
         <v>11</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>21</v>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2">
-        <v>41</v>
-      </c>
+      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2">
-        <v>51</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>61</v>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>71</v>
-      </c>
+      <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
     </row>
@@ -836,35 +790,38 @@
       <c r="A8" s="1">
         <v>30</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>21</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <v>41</v>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <v>51</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2">
-        <v>61</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
-        <v>71</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2">
-        <v>81</v>
-      </c>
-      <c r="P8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="Q8" s="2" t="s">
         <v>0</v>
       </c>
@@ -876,34 +833,38 @@
         <v>38</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>41</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>51</v>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2">
-        <v>61</v>
-      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2">
-        <v>71</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2">
-        <v>81</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2">
-        <v>91</v>
-      </c>
-      <c r="P9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="Q9" s="2" t="s">
         <v>0</v>
       </c>
@@ -916,30 +877,40 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
-        <v>51</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <v>61</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2">
-        <v>71</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2">
-        <v>81</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2">
-        <v>91</v>
-      </c>
-      <c r="O10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="P10" s="2" t="s">
         <v>0</v>
       </c>
@@ -951,73 +922,119 @@
       <c r="A11" s="1">
         <v>48</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2">
-        <v>61</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2">
-        <v>71</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2">
-        <v>81</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2">
-        <v>91</v>
-      </c>
-      <c r="M11" s="2"/>
+      <c r="B11" s="2">
+        <v>71</v>
+      </c>
+      <c r="C11" s="2">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2">
+        <v>71</v>
+      </c>
+      <c r="E11" s="2">
+        <v>71</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="N11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>71</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>71</v>
+      </c>
+      <c r="R11" s="2">
+        <v>71</v>
+      </c>
+      <c r="S11" s="2">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>50</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="B12" s="2">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2">
+        <v>71</v>
+      </c>
+      <c r="E12" s="2">
+        <v>71</v>
+      </c>
+      <c r="F12" s="2">
+        <v>71</v>
+      </c>
       <c r="G12" s="2">
         <v>71</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>71</v>
+      </c>
       <c r="I12" s="2">
-        <v>81</v>
-      </c>
-      <c r="J12" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="J12" s="2">
+        <v>71</v>
+      </c>
       <c r="K12" s="2">
-        <v>91</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="L12" s="2">
+        <v>71</v>
+      </c>
+      <c r="M12" s="2">
+        <v>71</v>
+      </c>
+      <c r="N12" s="2">
+        <v>71</v>
+      </c>
+      <c r="O12" s="2">
+        <v>71</v>
+      </c>
+      <c r="P12" s="2">
+        <v>71</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>71</v>
+      </c>
+      <c r="R12" s="2">
+        <v>71</v>
+      </c>
+      <c r="S12" s="2">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1027,25 +1044,15 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2">
-        <v>81</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2">
-        <v>91</v>
-      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1061,21 +1068,13 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1108,51 +1107,54 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:S15">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="between">
+    <cfRule type="beginsWith" dxfId="12" priority="1" operator="beginsWith" text="c">
+      <formula>LEFT(B2,LEN("c"))="c"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="2" operator="beginsWith" text="b">
+      <formula>LEFT(B2,LEN("b"))="b"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="10" priority="3" operator="beginsWith" text="a">
+      <formula>LEFT(B2,LEN("a"))="a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="between">
+      <formula>90</formula>
+      <formula>100</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="between">
+      <formula>80</formula>
+      <formula>90</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="between">
+      <formula>70</formula>
+      <formula>80</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
+      <formula>60</formula>
+      <formula>70</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="between">
+      <formula>50</formula>
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="between">
+      <formula>40</formula>
+      <formula>50</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="between">
+      <formula>30</formula>
+      <formula>40</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="between">
+      <formula>20</formula>
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="between">
+      <formula>10</formula>
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="between">
       <formula>1</formula>
       <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="between">
-      <formula>10</formula>
-      <formula>20</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="between">
-      <formula>20</formula>
-      <formula>30</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
-      <formula>30</formula>
-      <formula>40</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
-      <formula>40</formula>
-      <formula>50</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
-      <formula>50</formula>
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
-      <formula>60</formula>
-      <formula>70</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
-      <formula>70</formula>
-      <formula>80</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
-      <formula>80</formula>
-      <formula>90</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
-      <formula>90</formula>
-      <formula>100</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="a">
-      <formula>LEFT(B2,LEN("a"))="a"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="b">
-      <formula>LEFT(B2,LEN("b"))="b"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>